<commit_message>
changed a few things on the hardware list
changed hardware the complete size to 355x355x350, as most beds sold in the market are 355x355mm instead of 350x350mm. so i prefer to just add 5mm overrall, also i made a mistake and calculate just 14 bars of 585, and it was actually 16 bars, so i changed on the list to 16 bars of 590mm, also changed the sized on 2020 gantry to accomodate this changes.
</commit_message>
<xml_diff>
--- a/Voron Tower/Hardware List 350x350mm.xlsx
+++ b/Voron Tower/Hardware List 350x350mm.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sales\Documents\GitHub\VoronTower\Voron Tower\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAB3C0-A6BD-4B1C-8794-4A008D03A7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -346,27 +355,12 @@
     <t>4040 Series-10 350mm</t>
   </si>
   <si>
-    <t>4040 Series-10 505mm</t>
-  </si>
-  <si>
     <t>4040 Series-10 540mm</t>
   </si>
   <si>
-    <t>4040 Series-10 585mm</t>
-  </si>
-  <si>
     <t>4040 Series-10 600mm</t>
   </si>
   <si>
-    <t>Misumi HFSB5-2020-385</t>
-  </si>
-  <si>
-    <t>Misumi HFSB5-2020-470</t>
-  </si>
-  <si>
-    <t>Misumi HFSB5-2020-575</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -503,30 +497,46 @@
   </si>
   <si>
     <t>M4 Knurled Nut (DIN 466-B)</t>
+  </si>
+  <si>
+    <t>4040 Series-10 590mm</t>
+  </si>
+  <si>
+    <t>4040 Series-10 510mm</t>
+  </si>
+  <si>
+    <t>Misumi HFSB5-2020-580</t>
+  </si>
+  <si>
+    <t>Misumi HFSB5-2020-390</t>
+  </si>
+  <si>
+    <t>Misumi HFSB5-2020-475</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16.0"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -536,7 +546,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -564,7 +574,13 @@
     </fill>
   </fills>
   <borders count="6">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -578,8 +594,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -589,6 +607,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -597,80 +616,92 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -860,27 +891,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E157"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.25"/>
-    <col customWidth="1" min="2" max="2" width="18.63"/>
-    <col customWidth="1" min="3" max="3" width="47.38"/>
-    <col customWidth="1" min="4" max="4" width="5.13"/>
-    <col customWidth="1" min="5" max="5" width="11.63"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,14 +933,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -915,14 +951,14 @@
         <v>7</v>
       </c>
       <c r="D3" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E61" si="1">D3</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
+        <f t="shared" ref="E3:E61" si="0">D3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -933,14 +969,14 @@
         <v>9</v>
       </c>
       <c r="D4" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -951,14 +987,14 @@
         <v>10</v>
       </c>
       <c r="D5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -969,14 +1005,14 @@
         <v>11</v>
       </c>
       <c r="D6" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -987,14 +1023,14 @@
         <v>12</v>
       </c>
       <c r="D7" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -1005,14 +1041,14 @@
         <v>14</v>
       </c>
       <c r="D8" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1023,14 +1059,14 @@
         <v>15</v>
       </c>
       <c r="D9" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1041,14 +1077,14 @@
         <v>16</v>
       </c>
       <c r="D10" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1059,14 +1095,14 @@
         <v>17</v>
       </c>
       <c r="D11" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1077,14 +1113,14 @@
         <v>18</v>
       </c>
       <c r="D12" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
@@ -1095,14 +1131,14 @@
         <v>19</v>
       </c>
       <c r="D13" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1113,14 +1149,14 @@
         <v>20</v>
       </c>
       <c r="D14" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1131,14 +1167,14 @@
         <v>21</v>
       </c>
       <c r="D15" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1149,14 +1185,14 @@
         <v>22</v>
       </c>
       <c r="D16" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
@@ -1167,14 +1203,14 @@
         <v>23</v>
       </c>
       <c r="D17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
@@ -1185,14 +1221,14 @@
         <v>24</v>
       </c>
       <c r="D18" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
@@ -1203,14 +1239,14 @@
         <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>13</v>
       </c>
@@ -1221,14 +1257,14 @@
         <v>26</v>
       </c>
       <c r="D20" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
@@ -1239,14 +1275,14 @@
         <v>27</v>
       </c>
       <c r="D21" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
@@ -1257,14 +1293,14 @@
         <v>28</v>
       </c>
       <c r="D22" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E22" s="10">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
@@ -1275,14 +1311,14 @@
         <v>29</v>
       </c>
       <c r="D23" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>13</v>
       </c>
@@ -1293,14 +1329,14 @@
         <v>30</v>
       </c>
       <c r="D24" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>13</v>
       </c>
@@ -1311,14 +1347,14 @@
         <v>31</v>
       </c>
       <c r="D25" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
@@ -1329,14 +1365,14 @@
         <v>32</v>
       </c>
       <c r="D26" s="9">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>13</v>
       </c>
@@ -1347,14 +1383,14 @@
         <v>33</v>
       </c>
       <c r="D27" s="9">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="E27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
@@ -1365,14 +1401,14 @@
         <v>34</v>
       </c>
       <c r="D28" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
@@ -1383,14 +1419,14 @@
         <v>35</v>
       </c>
       <c r="D29" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1401,14 +1437,14 @@
         <v>36</v>
       </c>
       <c r="D30" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>13</v>
       </c>
@@ -1419,14 +1455,14 @@
         <v>37</v>
       </c>
       <c r="D31" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>13</v>
       </c>
@@ -1437,14 +1473,14 @@
         <v>38</v>
       </c>
       <c r="D32" s="9">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="E32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>13</v>
       </c>
@@ -1455,14 +1491,14 @@
         <v>39</v>
       </c>
       <c r="D33" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
@@ -1473,14 +1509,14 @@
         <v>40</v>
       </c>
       <c r="D34" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>41</v>
       </c>
@@ -1491,14 +1527,14 @@
         <v>42</v>
       </c>
       <c r="D35" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>41</v>
       </c>
@@ -1509,14 +1545,14 @@
         <v>43</v>
       </c>
       <c r="D36" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>41</v>
       </c>
@@ -1527,14 +1563,14 @@
         <v>44</v>
       </c>
       <c r="D37" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E37" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>41</v>
       </c>
@@ -1545,14 +1581,14 @@
         <v>45</v>
       </c>
       <c r="D38" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>41</v>
       </c>
@@ -1563,14 +1599,14 @@
         <v>46</v>
       </c>
       <c r="D39" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>41</v>
       </c>
@@ -1581,14 +1617,14 @@
         <v>47</v>
       </c>
       <c r="D40" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>41</v>
       </c>
@@ -1599,14 +1635,14 @@
         <v>48</v>
       </c>
       <c r="D41" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>41</v>
       </c>
@@ -1617,14 +1653,14 @@
         <v>49</v>
       </c>
       <c r="D42" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>41</v>
       </c>
@@ -1635,14 +1671,14 @@
         <v>50</v>
       </c>
       <c r="D43" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>41</v>
       </c>
@@ -1653,14 +1689,14 @@
         <v>51</v>
       </c>
       <c r="D44" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>41</v>
       </c>
@@ -1671,14 +1707,14 @@
         <v>52</v>
       </c>
       <c r="D45" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>41</v>
       </c>
@@ -1689,14 +1725,14 @@
         <v>53</v>
       </c>
       <c r="D46" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>41</v>
       </c>
@@ -1707,14 +1743,14 @@
         <v>54</v>
       </c>
       <c r="D47" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>41</v>
       </c>
@@ -1725,14 +1761,14 @@
         <v>55</v>
       </c>
       <c r="D48" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>41</v>
       </c>
@@ -1743,14 +1779,14 @@
         <v>56</v>
       </c>
       <c r="D49" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>41</v>
       </c>
@@ -1761,14 +1797,14 @@
         <v>57</v>
       </c>
       <c r="D50" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>41</v>
       </c>
@@ -1779,14 +1815,14 @@
         <v>58</v>
       </c>
       <c r="D51" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E51" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>41</v>
       </c>
@@ -1797,14 +1833,14 @@
         <v>59</v>
       </c>
       <c r="D52" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E52" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>41</v>
       </c>
@@ -1815,14 +1851,14 @@
         <v>60</v>
       </c>
       <c r="D53" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>41</v>
       </c>
@@ -1833,14 +1869,14 @@
         <v>61</v>
       </c>
       <c r="D54" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>41</v>
       </c>
@@ -1851,14 +1887,14 @@
         <v>62</v>
       </c>
       <c r="D55" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>41</v>
       </c>
@@ -1869,14 +1905,14 @@
         <v>63</v>
       </c>
       <c r="D56" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E56" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>41</v>
       </c>
@@ -1887,14 +1923,14 @@
         <v>64</v>
       </c>
       <c r="D57" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>41</v>
       </c>
@@ -1905,14 +1941,14 @@
         <v>65</v>
       </c>
       <c r="D58" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>41</v>
       </c>
@@ -1923,14 +1959,14 @@
         <v>66</v>
       </c>
       <c r="D59" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>41</v>
       </c>
@@ -1941,14 +1977,14 @@
         <v>67</v>
       </c>
       <c r="D60" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -1959,14 +1995,14 @@
         <v>69</v>
       </c>
       <c r="D61" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>68</v>
       </c>
@@ -1977,14 +2013,14 @@
         <v>70</v>
       </c>
       <c r="D62" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E62" s="7">
         <f>D62+D88</f>
         <v>29</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>68</v>
       </c>
@@ -1999,11 +2035,11 @@
         <v>96</v>
       </c>
       <c r="E63" s="7">
-        <f t="shared" ref="E63:E64" si="2">D63</f>
+        <f t="shared" ref="E63:E64" si="1">D63</f>
         <v>96</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>68</v>
       </c>
@@ -2018,11 +2054,11 @@
         <v>82</v>
       </c>
       <c r="E64" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>68</v>
       </c>
@@ -2033,14 +2069,14 @@
         <v>73</v>
       </c>
       <c r="D65" s="6">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="E65" s="7">
         <f>D65+D97-D143</f>
         <v>44</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>68</v>
       </c>
@@ -2051,14 +2087,14 @@
         <v>74</v>
       </c>
       <c r="D66" s="6">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="E66" s="7">
-        <f t="shared" ref="E66:E67" si="3">D66</f>
+        <f t="shared" ref="E66:E67" si="2">D66</f>
         <v>84</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>68</v>
       </c>
@@ -2069,14 +2105,14 @@
         <v>75</v>
       </c>
       <c r="D67" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="E67" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>68</v>
       </c>
@@ -2087,14 +2123,14 @@
         <v>76</v>
       </c>
       <c r="D68" s="6">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="E68" s="7">
         <f>D68+D99-D146</f>
         <v>22</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>68</v>
       </c>
@@ -2105,14 +2141,14 @@
         <v>77</v>
       </c>
       <c r="D69" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E69" s="7">
         <f>D69+D100</f>
         <v>26</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>68</v>
       </c>
@@ -2127,11 +2163,11 @@
         <v>4</v>
       </c>
       <c r="E70" s="7">
-        <f t="shared" ref="E70:E87" si="4">D70</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71">
+        <f t="shared" ref="E70:E87" si="3">D70</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>68</v>
       </c>
@@ -2146,11 +2182,11 @@
         <v>104</v>
       </c>
       <c r="E71" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>68</v>
       </c>
@@ -2165,11 +2201,11 @@
         <v>42</v>
       </c>
       <c r="E72" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>68</v>
       </c>
@@ -2180,14 +2216,14 @@
         <v>81</v>
       </c>
       <c r="D73" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E73" s="7">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>68</v>
       </c>
@@ -2198,14 +2234,14 @@
         <v>82</v>
       </c>
       <c r="D74" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E74" s="7">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>68</v>
       </c>
@@ -2220,11 +2256,11 @@
         <v>153</v>
       </c>
       <c r="E75" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>68</v>
       </c>
@@ -2235,14 +2271,14 @@
         <v>84</v>
       </c>
       <c r="D76" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E76" s="7">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>68</v>
       </c>
@@ -2253,14 +2289,14 @@
         <v>85</v>
       </c>
       <c r="D77" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E77" s="7">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>68</v>
       </c>
@@ -2271,319 +2307,319 @@
         <v>86</v>
       </c>
       <c r="D78" s="9">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="E78" s="10">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A79" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D79" s="9">
+        <v>60</v>
+      </c>
+      <c r="E79" s="10">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="9">
+        <v>6</v>
+      </c>
+      <c r="E80" s="10">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="9">
+        <v>103</v>
+      </c>
+      <c r="E81" s="10">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" s="9">
+        <v>110</v>
+      </c>
+      <c r="E82" s="10">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D83" s="9">
+        <v>3</v>
+      </c>
+      <c r="E83" s="10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D84" s="9">
+        <v>4</v>
+      </c>
+      <c r="E84" s="10">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="9">
+        <v>41</v>
+      </c>
+      <c r="E85" s="10">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="9">
+        <v>20</v>
+      </c>
+      <c r="E86" s="10">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" s="9">
+        <v>22</v>
+      </c>
+      <c r="E87" s="10">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" s="9">
+        <v>25</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D89" s="9">
+        <v>30</v>
+      </c>
+      <c r="E89" s="10">
+        <f t="shared" ref="E89:E96" si="4">D89</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D90" s="9">
+        <v>11</v>
+      </c>
+      <c r="E90" s="10">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="9">
+        <v>8</v>
+      </c>
+      <c r="E91" s="10">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" s="9">
+        <v>187</v>
+      </c>
+      <c r="E92" s="10">
+        <f t="shared" si="4"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="9">
+        <v>7</v>
+      </c>
+      <c r="E93" s="10">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A94" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="9">
+        <v>42</v>
+      </c>
+      <c r="E94" s="10">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D95" s="9">
+        <v>16</v>
+      </c>
+      <c r="E95" s="10">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D79" s="9">
-        <v>60.0</v>
-      </c>
-      <c r="E79" s="10">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E80" s="10">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D81" s="9">
-        <v>103.0</v>
-      </c>
-      <c r="E81" s="10">
-        <f t="shared" si="4"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D82" s="9">
-        <v>110.0</v>
-      </c>
-      <c r="E82" s="10">
-        <f t="shared" si="4"/>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D83" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="E83" s="10">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D84" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E84" s="10">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D85" s="9">
-        <v>41.0</v>
-      </c>
-      <c r="E85" s="10">
-        <f t="shared" si="4"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D86" s="9">
-        <v>20.0</v>
-      </c>
-      <c r="E86" s="10">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" s="9">
-        <v>22.0</v>
-      </c>
-      <c r="E87" s="10">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D88" s="9">
-        <v>25.0</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D89" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="E89" s="10">
-        <f t="shared" ref="E89:E96" si="5">D89</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D90" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="E90" s="10">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D91" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="E91" s="10">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D92" s="9">
-        <v>187.0</v>
-      </c>
-      <c r="E92" s="10">
-        <f t="shared" si="5"/>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D93" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="E93" s="10">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D94" s="9">
-        <v>42.0</v>
-      </c>
-      <c r="E94" s="10">
-        <f t="shared" si="5"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D95" s="9">
-        <v>16.0</v>
-      </c>
-      <c r="E95" s="10">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="96">
+    <row r="96" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
         <v>68</v>
       </c>
@@ -2594,14 +2630,14 @@
         <v>104</v>
       </c>
       <c r="D96" s="9">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="E96" s="10">
-        <f t="shared" si="5"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="97">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>68</v>
       </c>
@@ -2612,13 +2648,13 @@
         <v>105</v>
       </c>
       <c r="D97" s="9">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
         <v>68</v>
       </c>
@@ -2629,14 +2665,14 @@
         <v>106</v>
       </c>
       <c r="D98" s="9">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="E98" s="10">
         <f>D98</f>
         <v>35</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
         <v>68</v>
       </c>
@@ -2647,13 +2683,13 @@
         <v>76</v>
       </c>
       <c r="D99" s="9">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>68</v>
       </c>
@@ -2664,13 +2700,13 @@
         <v>107</v>
       </c>
       <c r="D100" s="9">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>108</v>
       </c>
@@ -2681,14 +2717,14 @@
         <v>109</v>
       </c>
       <c r="D101" s="6">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="E101" s="7">
-        <f t="shared" ref="E101:E140" si="6">D101</f>
+        <f t="shared" ref="E101:E140" si="5">D101</f>
         <v>72</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>108</v>
       </c>
@@ -2699,14 +2735,14 @@
         <v>110</v>
       </c>
       <c r="D102" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E102" s="7">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>108</v>
       </c>
@@ -2714,17 +2750,17 @@
         <v>6</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="D103" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E103" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>108</v>
       </c>
@@ -2732,17 +2768,17 @@
         <v>6</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D104" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E104" s="7">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>108</v>
       </c>
@@ -2750,17 +2786,17 @@
         <v>6</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="D105" s="6">
-        <v>14.0</v>
+        <v>16</v>
       </c>
       <c r="E105" s="7">
-        <f t="shared" si="6"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>108</v>
       </c>
@@ -2768,17 +2804,17 @@
         <v>6</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D106" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E106" s="7">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>108</v>
       </c>
@@ -2786,17 +2822,17 @@
         <v>6</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
       <c r="D107" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="7">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>108</v>
       </c>
@@ -2804,17 +2840,17 @@
         <v>6</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="D108" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="7">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>108</v>
       </c>
@@ -2822,597 +2858,597 @@
         <v>6</v>
       </c>
       <c r="C109" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D109" s="6">
+        <v>2</v>
+      </c>
+      <c r="E109" s="7">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D110" s="9">
+        <v>1</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A111" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D111" s="9">
+        <v>1</v>
+      </c>
+      <c r="E111" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D112" s="9">
+        <v>1</v>
+      </c>
+      <c r="E112" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D109" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="E109" s="7">
-        <f t="shared" si="6"/>
+      <c r="D113" s="9">
+        <v>1</v>
+      </c>
+      <c r="E113" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="9">
+        <v>1</v>
+      </c>
+      <c r="E114" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D115" s="9">
+        <v>8</v>
+      </c>
+      <c r="E115" s="10">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D116" s="9">
+        <v>1</v>
+      </c>
+      <c r="E116" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D117" s="9">
+        <v>1</v>
+      </c>
+      <c r="E117" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A118" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D118" s="9">
+        <v>1</v>
+      </c>
+      <c r="E118" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D119" s="9">
+        <v>1</v>
+      </c>
+      <c r="E119" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D120" s="9">
+        <v>12</v>
+      </c>
+      <c r="E120" s="10">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A121" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" s="9">
+        <v>1</v>
+      </c>
+      <c r="E121" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D122" s="9">
+        <v>20</v>
+      </c>
+      <c r="E122" s="10">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D123" s="9">
+        <v>4</v>
+      </c>
+      <c r="E123" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A124" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D124" s="9">
+        <v>3</v>
+      </c>
+      <c r="E124" s="10">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A125" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D125" s="9">
+        <v>4</v>
+      </c>
+      <c r="E125" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A126" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D126" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D110" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E110" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D111" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E111" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D112" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E112" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D113" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E113" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C114" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D114" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E114" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C115" s="9" t="s">
+      <c r="E126" s="10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D115" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="E115" s="10">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C116" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D116" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E116" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D117" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E117" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D118" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E118" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D119" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E119" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C120" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D120" s="9">
-        <v>12.0</v>
-      </c>
-      <c r="E120" s="10">
-        <f t="shared" si="6"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D121" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E121" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C122" s="9" t="s">
+      <c r="B127" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D122" s="9">
-        <v>20.0</v>
-      </c>
-      <c r="E122" s="10">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" s="9" t="s">
+      <c r="D127" s="9">
+        <v>4</v>
+      </c>
+      <c r="E127" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D123" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E123" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C124" s="9" t="s">
+      <c r="D128" s="9">
+        <v>4</v>
+      </c>
+      <c r="E128" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A129" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D124" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="E124" s="10">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C125" s="9" t="s">
+      <c r="D129" s="9">
+        <v>4</v>
+      </c>
+      <c r="E129" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A130" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D125" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E125" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C126" s="9" t="s">
+      <c r="D130" s="9">
+        <v>2</v>
+      </c>
+      <c r="E130" s="10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A131" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D126" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E126" s="10">
-        <f t="shared" si="6"/>
+      <c r="D131" s="9">
+        <v>4</v>
+      </c>
+      <c r="E131" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A132" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D132" s="9">
+        <v>1</v>
+      </c>
+      <c r="E132" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A133" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D133" s="9">
+        <v>6</v>
+      </c>
+      <c r="E133" s="10">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A134" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D134" s="9">
+        <v>1</v>
+      </c>
+      <c r="E134" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A135" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D135" s="9">
+        <v>4</v>
+      </c>
+      <c r="E135" s="10">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A136" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D136" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D127" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E127" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D128" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E128" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B129" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D129" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E129" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C130" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D130" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E130" s="10">
-        <f t="shared" si="6"/>
+      <c r="E136" s="10">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C131" s="9" t="s">
+    <row r="137" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A137" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D131" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E131" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D132" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E132" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C133" s="9" t="s">
+      <c r="B137" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D133" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E133" s="10">
-        <f t="shared" si="6"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B134" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134" s="9" t="s">
+      <c r="D137" s="9">
+        <v>1</v>
+      </c>
+      <c r="E137" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A138" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D134" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E134" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C135" s="9" t="s">
+      <c r="D138" s="9">
+        <v>2</v>
+      </c>
+      <c r="E138" s="10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A139" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D135" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E135" s="10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="8" t="s">
+      <c r="D139" s="9">
+        <v>2</v>
+      </c>
+      <c r="E139" s="10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A140" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B136" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="9" t="s">
+      <c r="D140" s="9">
+        <v>1</v>
+      </c>
+      <c r="E140" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A141" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B141" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="D136" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E136" s="10">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D137" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E137" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B138" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D138" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E138" s="10">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D139" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="E139" s="10">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C140" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D140" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="E140" s="10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B141" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D141" s="12">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="E141" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>100</v>
@@ -3425,29 +3461,29 @@
         <v>96</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>105</v>
       </c>
       <c r="D143" s="12">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E143" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>106</v>
@@ -3460,12 +3496,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>95</v>
@@ -3478,12 +3514,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>76</v>
@@ -3496,194 +3532,194 @@
         <v>96</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D147" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E147" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D148" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E148" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D149" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E149" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D150" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E150" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B151" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C151" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C151" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="D151" s="12">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E151" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D152" s="12">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E152" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D153" s="12">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E153" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D154" s="12">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E154" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D155" s="12">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E155" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="11" t="s">
         <v>108</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D156" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E156" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D157" s="12">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E157" s="13" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Hardware List 350x350mm.xlsx
changed feet to 640mm instead of 600mm
</commit_message>
<xml_diff>
--- a/Voron Tower/Hardware List 350x350mm.xlsx
+++ b/Voron Tower/Hardware List 350x350mm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sales\Documents\GitHub\VoronTower\Voron Tower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDAB3C0-A6BD-4B1C-8794-4A008D03A7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFED34E5-7A95-421C-A7B9-DA0DC79F31D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,9 +358,6 @@
     <t>4040 Series-10 540mm</t>
   </si>
   <si>
-    <t>4040 Series-10 600mm</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -512,6 +509,9 @@
   </si>
   <si>
     <t>Misumi HFSB5-2020-475</t>
+  </si>
+  <si>
+    <t>4040 Series-10 640mm</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -933,14 +933,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -958,7 +958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>13</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>13</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>13</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>13</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>13</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>13</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>41</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>41</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>6</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D103" s="6">
         <v>2</v>
@@ -2786,7 +2786,7 @@
         <v>6</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D105" s="6">
         <v>16</v>
@@ -2804,7 +2804,7 @@
         <v>6</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="D106" s="6">
         <v>4</v>
@@ -2822,7 +2822,7 @@
         <v>6</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D107" s="6">
         <v>1</v>
@@ -2840,7 +2840,7 @@
         <v>6</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D108" s="6">
         <v>1</v>
@@ -2858,7 +2858,7 @@
         <v>6</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D109" s="6">
         <v>2</v>
@@ -2870,13 +2870,13 @@
     </row>
     <row r="110" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="D110" s="9">
         <v>1</v>
@@ -2888,13 +2888,13 @@
     </row>
     <row r="111" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D111" s="9">
         <v>1</v>
@@ -2906,13 +2906,13 @@
     </row>
     <row r="112" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D112" s="9">
         <v>1</v>
@@ -2924,13 +2924,13 @@
     </row>
     <row r="113" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D113" s="9">
         <v>1</v>
@@ -2942,13 +2942,13 @@
     </row>
     <row r="114" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D114" s="9">
         <v>1</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="115" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D115" s="9">
         <v>8</v>
@@ -2978,13 +2978,13 @@
     </row>
     <row r="116" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B116" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D116" s="9">
         <v>1</v>
@@ -2996,13 +2996,13 @@
     </row>
     <row r="117" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B117" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D117" s="9">
         <v>1</v>
@@ -3014,13 +3014,13 @@
     </row>
     <row r="118" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B118" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D118" s="9">
         <v>1</v>
@@ -3032,13 +3032,13 @@
     </row>
     <row r="119" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B119" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D119" s="9">
         <v>1</v>
@@ -3050,13 +3050,13 @@
     </row>
     <row r="120" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C120" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D120" s="9">
         <v>12</v>
@@ -3068,13 +3068,13 @@
     </row>
     <row r="121" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D121" s="9">
         <v>1</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="122" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B122" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D122" s="9">
         <v>20</v>
@@ -3104,13 +3104,13 @@
     </row>
     <row r="123" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D123" s="9">
         <v>4</v>
@@ -3122,13 +3122,13 @@
     </row>
     <row r="124" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D124" s="9">
         <v>3</v>
@@ -3140,13 +3140,13 @@
     </row>
     <row r="125" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D125" s="9">
         <v>4</v>
@@ -3158,13 +3158,13 @@
     </row>
     <row r="126" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D126" s="9">
         <v>2</v>
@@ -3176,13 +3176,13 @@
     </row>
     <row r="127" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A127" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D127" s="9">
         <v>4</v>
@@ -3194,13 +3194,13 @@
     </row>
     <row r="128" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B128" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D128" s="9">
         <v>4</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="129" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B129" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D129" s="9">
         <v>4</v>
@@ -3230,13 +3230,13 @@
     </row>
     <row r="130" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B130" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D130" s="9">
         <v>2</v>
@@ -3248,13 +3248,13 @@
     </row>
     <row r="131" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B131" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D131" s="9">
         <v>4</v>
@@ -3266,13 +3266,13 @@
     </row>
     <row r="132" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B132" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D132" s="9">
         <v>1</v>
@@ -3284,13 +3284,13 @@
     </row>
     <row r="133" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B133" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D133" s="9">
         <v>6</v>
@@ -3302,13 +3302,13 @@
     </row>
     <row r="134" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B134" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D134" s="9">
         <v>1</v>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="135" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B135" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D135" s="9">
         <v>4</v>
@@ -3338,13 +3338,13 @@
     </row>
     <row r="136" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="D136" s="9">
         <v>2</v>
@@ -3356,13 +3356,13 @@
     </row>
     <row r="137" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D137" s="9">
         <v>1</v>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="138" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D138" s="9">
         <v>2</v>
@@ -3392,13 +3392,13 @@
     </row>
     <row r="139" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A139" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B139" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D139" s="9">
         <v>2</v>
@@ -3410,13 +3410,13 @@
     </row>
     <row r="140" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D140" s="9">
         <v>1</v>
@@ -3431,7 +3431,7 @@
         <v>68</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>93</v>
@@ -3448,7 +3448,7 @@
         <v>68</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>100</v>
@@ -3466,7 +3466,7 @@
         <v>68</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>105</v>
@@ -3483,7 +3483,7 @@
         <v>68</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>106</v>
@@ -3501,7 +3501,7 @@
         <v>68</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>95</v>
@@ -3519,7 +3519,7 @@
         <v>68</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>76</v>
@@ -3537,10 +3537,10 @@
         <v>68</v>
       </c>
       <c r="B147" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C147" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="C147" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="D147" s="12">
         <v>4</v>
@@ -3554,7 +3554,7 @@
         <v>68</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>88</v>
@@ -3568,13 +3568,13 @@
     </row>
     <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C149" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="B149" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C149" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="D149" s="12">
         <v>4</v>
@@ -3588,10 +3588,10 @@
         <v>108</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D150" s="12">
         <v>4</v>
@@ -3605,10 +3605,10 @@
         <v>108</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D151" s="12">
         <v>1</v>
@@ -3622,10 +3622,10 @@
         <v>108</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D152" s="12">
         <v>2</v>
@@ -3639,10 +3639,10 @@
         <v>108</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D153" s="12">
         <v>1</v>
@@ -3656,10 +3656,10 @@
         <v>108</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D154" s="12">
         <v>2</v>
@@ -3673,10 +3673,10 @@
         <v>108</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D155" s="12">
         <v>10</v>
@@ -3690,10 +3690,10 @@
         <v>108</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D156" s="12">
         <v>4</v>
@@ -3707,10 +3707,10 @@
         <v>68</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D157" s="12">
         <v>4</v>

</xml_diff>